<commit_message>
Before discussion with gls
</commit_message>
<xml_diff>
--- a/LCOH_calculation/lcoh_model.xlsx
+++ b/LCOH_calculation/lcoh_model.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\LCOH_calculation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhD\H2_gui\LCOH_calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9084" windowHeight="6696"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9090" windowHeight="6690"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -399,15 +399,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J87"/>
+  <dimension ref="A1:K87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -427,7 +427,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -454,15 +454,19 @@
         <v>0.20000000000000018</v>
       </c>
       <c r="I2">
-        <f>H2/B2</f>
-        <v>6.8965517241379379E-2</v>
+        <f>H2/B2*100</f>
+        <v>6.8965517241379377</v>
       </c>
       <c r="J2">
         <f>AVERAGE(I2:I87)</f>
-        <v>9.9866337972863498E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>9.9866337972863448</v>
+      </c>
+      <c r="K2">
+        <f>AVERAGE(H2:H88)</f>
+        <v>0.3096511627906976</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -489,11 +493,11 @@
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I66" si="1">H3/B3</f>
-        <v>1.5228426395939101E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <f t="shared" ref="I3:I66" si="1">H3/B3*100</f>
+        <v>1.5228426395939101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -521,10 +525,10 @@
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
-        <v>0.35714285714285721</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>35.714285714285722</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -552,10 +556,10 @@
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>5.2631578947368578E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>5.2631578947368576</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -583,10 +587,10 @@
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>6.4150943396226387E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>6.4150943396226383</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -614,10 +618,10 @@
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
-        <v>2.7027027027026848E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>2.7027027027026849</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -645,10 +649,10 @@
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
-        <v>6.8376068376068438E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>6.8376068376068435</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -676,10 +680,10 @@
       </c>
       <c r="I9">
         <f t="shared" si="1"/>
-        <v>0.23747276688453156</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>23.747276688453155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -707,10 +711,10 @@
       </c>
       <c r="I10">
         <f t="shared" si="1"/>
-        <v>7.880434782608696E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <v>7.8804347826086962</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -738,10 +742,10 @@
       </c>
       <c r="I11">
         <f t="shared" si="1"/>
-        <v>3.6269430051813503E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>3.6269430051813503</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -769,10 +773,10 @@
       </c>
       <c r="I12">
         <f t="shared" si="1"/>
-        <v>0.10946745562130181</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <v>10.946745562130181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -800,10 +804,10 @@
       </c>
       <c r="I13">
         <f t="shared" si="1"/>
-        <v>0.18691588785046723</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+        <v>18.691588785046722</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -831,10 +835,10 @@
       </c>
       <c r="I14">
         <f t="shared" si="1"/>
-        <v>0.21052631578947364</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+        <v>21.052631578947363</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -862,10 +866,10 @@
       </c>
       <c r="I15">
         <f t="shared" si="1"/>
-        <v>4.3668122270741428E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.43668122270741427</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -893,10 +897,10 @@
       </c>
       <c r="I16">
         <f t="shared" si="1"/>
-        <v>0.11254019292604504</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>11.254019292604504</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -924,10 +928,10 @@
       </c>
       <c r="I17">
         <f t="shared" si="1"/>
-        <v>4.2968749999999951E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.2968749999999956</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -955,10 +959,10 @@
       </c>
       <c r="I18">
         <f t="shared" si="1"/>
-        <v>6.7796610169491428E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+        <v>6.7796610169491425</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -986,10 +990,10 @@
       </c>
       <c r="I19">
         <f t="shared" si="1"/>
-        <v>0.12711864406779674</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+        <v>12.711864406779675</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1017,10 +1021,10 @@
       </c>
       <c r="I20">
         <f t="shared" si="1"/>
-        <v>0.19730941704035873</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+        <v>19.730941704035875</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1048,10 +1052,10 @@
       </c>
       <c r="I21">
         <f t="shared" si="1"/>
-        <v>0.12807881773399027</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+        <v>12.807881773399027</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1079,10 +1083,10 @@
       </c>
       <c r="I22">
         <f t="shared" si="1"/>
-        <v>0.10035842293906803</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+        <v>10.035842293906803</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1110,10 +1114,10 @@
       </c>
       <c r="I23">
         <f t="shared" si="1"/>
-        <v>6.0975609756097622E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+        <v>6.0975609756097624</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1141,10 +1145,10 @@
       </c>
       <c r="I24">
         <f t="shared" si="1"/>
-        <v>6.8111455108359198E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+        <v>6.81114551083592</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1172,10 +1176,10 @@
       </c>
       <c r="I25">
         <f t="shared" si="1"/>
-        <v>9.6774193548387039E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9.6774193548387046</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1203,10 +1207,10 @@
       </c>
       <c r="I26">
         <f t="shared" si="1"/>
-        <v>0.23893805309734517</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+        <v>23.893805309734518</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1234,10 +1238,10 @@
       </c>
       <c r="I27">
         <f t="shared" si="1"/>
-        <v>4.0909090909090839E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.0909090909090837</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1265,10 +1269,10 @@
       </c>
       <c r="I28">
         <f t="shared" si="1"/>
-        <v>0.17977528089887634</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+        <v>17.977528089887635</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1296,10 +1300,10 @@
       </c>
       <c r="I29">
         <f t="shared" si="1"/>
-        <v>0.10839160839160841</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+        <v>10.839160839160842</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1327,10 +1331,10 @@
       </c>
       <c r="I30">
         <f t="shared" si="1"/>
-        <v>4.3956043956043994E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.3956043956043995</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1358,10 +1362,10 @@
       </c>
       <c r="I31">
         <f t="shared" si="1"/>
-        <v>0.2088974854932302</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+        <v>20.88974854932302</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1389,10 +1393,10 @@
       </c>
       <c r="I32">
         <f t="shared" si="1"/>
-        <v>2.5641025641025664E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2.5641025641025665</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1420,10 +1424,10 @@
       </c>
       <c r="I33">
         <f t="shared" si="1"/>
-        <v>8.2901554404145039E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8.2901554404145035</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1451,10 +1455,10 @@
       </c>
       <c r="I34">
         <f t="shared" si="1"/>
-        <v>7.9812206572769925E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+        <v>7.9812206572769924</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1482,10 +1486,10 @@
       </c>
       <c r="I35">
         <f t="shared" si="1"/>
-        <v>9.5693779904306317E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9.5693779904306311</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1513,10 +1517,10 @@
       </c>
       <c r="I36">
         <f t="shared" si="1"/>
-        <v>5.8558558558558509E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5.8558558558558511</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1544,10 +1548,10 @@
       </c>
       <c r="I37">
         <f t="shared" si="1"/>
-        <v>4.8076923076923121E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.8076923076923119</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1575,10 +1579,10 @@
       </c>
       <c r="I38">
         <f t="shared" si="1"/>
-        <v>6.6433566433566418E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+        <v>6.6433566433566416</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1606,10 +1610,10 @@
       </c>
       <c r="I39">
         <f t="shared" si="1"/>
-        <v>6.6202090592334478E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+        <v>6.6202090592334475</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1637,10 +1641,10 @@
       </c>
       <c r="I40">
         <f t="shared" si="1"/>
-        <v>0.17227722772277229</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+        <v>17.227722772277229</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1668,10 +1672,10 @@
       </c>
       <c r="I41">
         <f t="shared" si="1"/>
-        <v>0.17721518987341769</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+        <v>17.721518987341771</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1699,10 +1703,10 @@
       </c>
       <c r="I42">
         <f t="shared" si="1"/>
-        <v>5.1282051282051329E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5.1282051282051331</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1730,10 +1734,10 @@
       </c>
       <c r="I43">
         <f t="shared" si="1"/>
-        <v>9.2307692307692271E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9.2307692307692264</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1761,10 +1765,10 @@
       </c>
       <c r="I44">
         <f t="shared" si="1"/>
-        <v>0.24183976261127582</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+        <v>24.183976261127583</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1792,10 +1796,10 @@
       </c>
       <c r="I45">
         <f t="shared" si="1"/>
-        <v>0.10106382978723402</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+        <v>10.106382978723403</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1823,10 +1827,10 @@
       </c>
       <c r="I46">
         <f t="shared" si="1"/>
-        <v>5.8091286307053805E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5.8091286307053807</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1854,10 +1858,10 @@
       </c>
       <c r="I47">
         <f t="shared" si="1"/>
-        <v>9.2307692307692271E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9.2307692307692264</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1885,10 +1889,10 @@
       </c>
       <c r="I48">
         <f t="shared" si="1"/>
-        <v>0.11707317073170743</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+        <v>11.707317073170744</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1916,10 +1920,10 @@
       </c>
       <c r="I49">
         <f t="shared" si="1"/>
-        <v>7.6190476190476045E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+        <v>7.6190476190476044</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1947,10 +1951,10 @@
       </c>
       <c r="I50">
         <f t="shared" si="1"/>
-        <v>0.12328767123287672</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+        <v>12.328767123287673</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1978,10 +1982,10 @@
       </c>
       <c r="I51">
         <f t="shared" si="1"/>
-        <v>0.10242587601078164</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+        <v>10.242587601078164</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2009,10 +2013,10 @@
       </c>
       <c r="I52">
         <f t="shared" si="1"/>
-        <v>3.0303030303030328E-2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+        <v>3.0303030303030329</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2040,10 +2044,10 @@
       </c>
       <c r="I53">
         <f t="shared" si="1"/>
-        <v>5.4347826086956652E-2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5.4347826086956648</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2071,10 +2075,10 @@
       </c>
       <c r="I54">
         <f t="shared" si="1"/>
-        <v>7.6470588235294193E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+        <v>7.6470588235294192</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2102,10 +2106,10 @@
       </c>
       <c r="I55">
         <f t="shared" si="1"/>
-        <v>0.12297734627831727</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+        <v>12.297734627831728</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2133,10 +2137,10 @@
       </c>
       <c r="I56">
         <f t="shared" si="1"/>
-        <v>0.11377245508982047</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+        <v>11.377245508982046</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2164,10 +2168,10 @@
       </c>
       <c r="I57">
         <f t="shared" si="1"/>
-        <v>0.22916666666666666</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+        <v>22.916666666666664</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2195,10 +2199,10 @@
       </c>
       <c r="I58">
         <f t="shared" si="1"/>
-        <v>9.3103448275862075E-2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9.3103448275862082</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2226,10 +2230,10 @@
       </c>
       <c r="I59">
         <f t="shared" si="1"/>
-        <v>9.3425605536332182E-2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9.3425605536332181</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2257,10 +2261,10 @@
       </c>
       <c r="I60">
         <f t="shared" si="1"/>
-        <v>0.12999999999999989</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+        <v>12.999999999999989</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2288,10 +2292,10 @@
       </c>
       <c r="I61">
         <f t="shared" si="1"/>
-        <v>4.035874439461877E-2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.0358744394618773</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2319,10 +2323,10 @@
       </c>
       <c r="I62">
         <f t="shared" si="1"/>
-        <v>2.1645021645021568E-2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2.1645021645021569</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2350,10 +2354,10 @@
       </c>
       <c r="I63">
         <f t="shared" si="1"/>
-        <v>0.12797619047619052</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+        <v>12.797619047619053</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2381,10 +2385,10 @@
       </c>
       <c r="I64">
         <f t="shared" si="1"/>
-        <v>0.10491803278688534</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+        <v>10.491803278688534</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2412,10 +2416,10 @@
       </c>
       <c r="I65">
         <f t="shared" si="1"/>
-        <v>8.7662337662337664E-2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8.7662337662337659</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2443,10 +2447,10 @@
       </c>
       <c r="I66">
         <f t="shared" si="1"/>
-        <v>0.10309278350515473</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+        <v>10.309278350515473</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2473,11 +2477,11 @@
         <v>0.16999999999999993</v>
       </c>
       <c r="I67">
-        <f t="shared" ref="I67:I87" si="3">H67/B67</f>
-        <v>5.7627118644067769E-2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+        <f t="shared" ref="I67:I87" si="3">H67/B67*100</f>
+        <v>5.7627118644067767</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2505,10 +2509,10 @@
       </c>
       <c r="I68">
         <f t="shared" si="3"/>
-        <v>4.0145985401459805E-2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.0145985401459807</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2536,10 +2540,10 @@
       </c>
       <c r="I69">
         <f t="shared" si="3"/>
-        <v>8.6092715231788006E-2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8.6092715231788013</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2567,10 +2571,10 @@
       </c>
       <c r="I70">
         <f t="shared" si="3"/>
-        <v>9.3841642228738947E-2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9.3841642228738955</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2598,10 +2602,10 @@
       </c>
       <c r="I71">
         <f t="shared" si="3"/>
-        <v>0.11444141689373295</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+        <v>11.444141689373295</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2629,10 +2633,10 @@
       </c>
       <c r="I72">
         <f t="shared" si="3"/>
-        <v>6.5934065934065991E-2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+        <v>6.5934065934065993</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2660,10 +2664,10 @@
       </c>
       <c r="I73">
         <f t="shared" si="3"/>
-        <v>7.6923076923076816E-2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+        <v>7.6923076923076819</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2691,10 +2695,10 @@
       </c>
       <c r="I74">
         <f t="shared" si="3"/>
-        <v>0.15274463007159894</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+        <v>15.274463007159895</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -2722,10 +2726,10 @@
       </c>
       <c r="I75">
         <f t="shared" si="3"/>
-        <v>9.7112860892388367E-2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+        <v>9.7112860892388362</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -2753,10 +2757,10 @@
       </c>
       <c r="I76">
         <f t="shared" si="3"/>
-        <v>8.8757396449704221E-2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8.8757396449704213</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -2784,10 +2788,10 @@
       </c>
       <c r="I77">
         <f t="shared" si="3"/>
-        <v>0.16414686825053992</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+        <v>16.414686825053991</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2815,10 +2819,10 @@
       </c>
       <c r="I78">
         <f t="shared" si="3"/>
-        <v>0.11061946902654868</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+        <v>11.061946902654867</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -2846,10 +2850,10 @@
       </c>
       <c r="I79">
         <f t="shared" si="3"/>
-        <v>0.12105263157894737</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+        <v>12.105263157894736</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -2877,10 +2881,10 @@
       </c>
       <c r="I80">
         <f t="shared" si="3"/>
-        <v>1.0989010989010999E-2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1.0989010989010999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2908,10 +2912,10 @@
       </c>
       <c r="I81">
         <f t="shared" si="3"/>
-        <v>4.3137254901960916E-2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.3137254901960915</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2939,10 +2943,10 @@
       </c>
       <c r="I82">
         <f t="shared" si="3"/>
-        <v>8.7323943661971853E-2</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8.7323943661971857</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2970,10 +2974,10 @@
       </c>
       <c r="I83">
         <f t="shared" si="3"/>
-        <v>1.4925373134328483E-2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1.4925373134328483</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -3001,10 +3005,10 @@
       </c>
       <c r="I84">
         <f t="shared" si="3"/>
-        <v>4.1420118343195304E-2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.14201183431953</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -3032,10 +3036,10 @@
       </c>
       <c r="I85">
         <f t="shared" si="3"/>
-        <v>0.11436950146627556</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+        <v>11.436950146627556</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -3063,10 +3067,10 @@
       </c>
       <c r="I86">
         <f t="shared" si="3"/>
-        <v>0.14832535885167467</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+        <v>14.832535885167466</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -3094,7 +3098,7 @@
       </c>
       <c r="I87">
         <f t="shared" si="3"/>
-        <v>0.16042780748663091</v>
+        <v>16.042780748663091</v>
       </c>
     </row>
   </sheetData>

</xml_diff>